<commit_message>
Updated the Summary data tab: if no CC starting with 27, the 2nd pivot table can't be filtered.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Recharges_Performer_VodafoneUsage\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A2C84-5AD4-4BFD-A2B2-62E81F65603A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC039260-D722-4A22-811C-F934636C7BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="23040" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -473,6 +473,30 @@
   </si>
   <si>
     <t>PivotTable1</t>
+  </si>
+  <si>
+    <t>Data\ExtendFormula.txt</t>
+  </si>
+  <si>
+    <t>vbaExtendFormulaCode</t>
+  </si>
+  <si>
+    <t>Data\CopyColumnDataInRange.txt</t>
+  </si>
+  <si>
+    <t>vbaCopyColumnDataInRangeCode</t>
+  </si>
+  <si>
+    <t>vbaRemoveDuplicatesInColumnCode</t>
+  </si>
+  <si>
+    <t>Data\RemoveDuplicatesInColumn.txt</t>
+  </si>
+  <si>
+    <t>Data\ExcludeSpecificValueInPivot.txt</t>
+  </si>
+  <si>
+    <t>vbaExcludeSpecificValueInPivotCode</t>
   </si>
 </sst>
 </file>
@@ -864,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1352,24 +1376,52 @@
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>146</v>
+      </c>
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A65" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A66" t="s">
+        <v>152</v>
+      </c>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>

</xml_diff>